<commit_message>
small update to use gsed on mac (homebrew install gnu-sed) as slightly different operation on mac.  TODO change this to a config (os=macos, windows,…)
</commit_message>
<xml_diff>
--- a/app1/app1.xlsx
+++ b/app1/app1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,8 @@
     <sheet name="User" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Patient" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Result" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="ability" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="config" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="286">
   <si>
     <t xml:space="preserve">status</t>
   </si>
@@ -556,6 +558,24 @@
     <t xml:space="preserve">f</t>
   </si>
   <si>
+    <t xml:space="preserve">Nathalia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tapia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fisher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bartlett</t>
+  </si>
+  <si>
     <t xml:space="preserve">Julianna</t>
   </si>
   <si>
@@ -773,6 +793,99 @@
   </si>
   <si>
     <t xml:space="preserve">Justice fortune no to is if winding morning forming.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business, Consumable, Device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read, update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient, Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clinic_admin_role, clinic_user_role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adapter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postgresql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">could be mysql or other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">localhost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">could be your ip address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blog_role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database login, must be set up in database prior to running script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  “      needs create database privileges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app_admin_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how the super admin will log into the web app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app_admin_password</t>
   </si>
 </sst>
 </file>
@@ -786,7 +899,7 @@
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="168" formatCode="MM/DD/YYYY\ HH:MM:SS"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -829,6 +942,14 @@
       <color rgb="FF000000"/>
       <name val="Courier 10 Pitch"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -877,7 +998,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -948,6 +1069,22 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1036,9 +1173,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.5263157894737"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.66801619433198"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8947368421053"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.78947368421053"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,18 +1240,18 @@
   <dimension ref="A1:K65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.336032388664"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.4008097165992"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.1943319838057"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.9514170040486"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.3198380566802"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.753036437247"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.9514170040486"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.8947368421053"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.6882591093117"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.1781376518219"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,8 +1686,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.66801619433198"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="23.6315789473684"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.78947368421053"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1581,11 +1718,11 @@
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>97BE-7540-27B3-6314</v>
+        <v>9C18-B31F-2966-27E0</v>
       </c>
       <c r="C3" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43214.2866878474</v>
+        <v>43212.5809094434</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,11 +1731,11 @@
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>368E-9A9F-730B-6A65</v>
+        <v>25B6-B096-D2EA-D278</v>
       </c>
       <c r="C4" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43147.2956499281</v>
+        <v>43545.5223033</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1607,11 +1744,11 @@
       </c>
       <c r="B5" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>A9DA-50B6-4FC-F922</v>
+        <v>C66C-847B-C388-F82F</v>
       </c>
       <c r="C5" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43621.0856335049</v>
+        <v>43158.8662442794</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1620,11 +1757,11 @@
       </c>
       <c r="B6" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>F440-DDB4-D52-45BE</v>
+        <v>18C2-271E-5C9-FA3B</v>
       </c>
       <c r="C6" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>42816.2233436504</v>
+        <v>42790.3158333455</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1633,11 +1770,11 @@
       </c>
       <c r="B7" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>9095-D305-5A5E-6CAE</v>
+        <v>DF2F-17E6-DBD9-8F8A</v>
       </c>
       <c r="C7" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43501.8750352257</v>
+        <v>43684.9756922602</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1646,11 +1783,11 @@
       </c>
       <c r="B8" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>CA03-D6C7-9D20-2A79</v>
+        <v>8B97-D15E-115-88CA</v>
       </c>
       <c r="C8" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>42962.8776223203</v>
+        <v>43041.8129668896</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1659,11 +1796,11 @@
       </c>
       <c r="B9" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>1B56-AB7C-212B-CDBF</v>
+        <v>1E42-6D03-CB2E-A0CD</v>
       </c>
       <c r="C9" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43451.7693923469</v>
+        <v>43327.4169632939</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,11 +1809,11 @@
       </c>
       <c r="B10" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>A5F8-26FC-87C7-F59B</v>
+        <v>2CEE-43E4-A139-2CAC</v>
       </c>
       <c r="C10" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43726.3133054519</v>
+        <v>43556.4409887449</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,11 +1822,11 @@
       </c>
       <c r="B11" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>C8A4-BCF9-E0E-11BD</v>
+        <v>663F-C9EC-BD79-E5D</v>
       </c>
       <c r="C11" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43276.7802612102</v>
+        <v>43529.0756262013</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1698,11 +1835,11 @@
       </c>
       <c r="B12" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>8AD2-325C-A9E3-A30F</v>
+        <v>43BC-D0E5-8355-762</v>
       </c>
       <c r="C12" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>42958.7297771376</v>
+        <v>43135.4908833929</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,11 +1848,11 @@
       </c>
       <c r="B13" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>72B8-551C-22B5-EFF1</v>
+        <v>126D-62D4-1FD1-BED5</v>
       </c>
       <c r="C13" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43657.2665788413</v>
+        <v>43666.2183029823</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,11 +1861,11 @@
       </c>
       <c r="B14" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>DA40-26FD-FB59-4CEC</v>
+        <v>E088-E635-AA76-CDA0</v>
       </c>
       <c r="C14" s="1" t="n">
         <f aca="true">NOW() +RAND()*1000</f>
-        <v>43743.2248074619</v>
+        <v>43671.9161165643</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1737,11 +1874,11 @@
       </c>
       <c r="B15" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>A97-FC5-F725-1C6E</v>
+        <v>E24B-6A9C-A91D-5690</v>
       </c>
       <c r="C15" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,11 +1887,11 @@
       </c>
       <c r="B16" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>8775-B212-96E9-AD70</v>
+        <v>EAE2-22E0-7BF0-9350</v>
       </c>
       <c r="C16" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1763,11 +1900,11 @@
       </c>
       <c r="B17" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>B605-FFC4-DA68-AAAD</v>
+        <v>4F16-2AD6-B854-6954</v>
       </c>
       <c r="C17" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,11 +1913,11 @@
       </c>
       <c r="B18" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>1B4E-97C0-370E-BFA9</v>
+        <v>A7-7483-C9E8-7032</v>
       </c>
       <c r="C18" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1789,11 +1926,11 @@
       </c>
       <c r="B19" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>E7C4-A81E-C105-6A81</v>
+        <v>7-4EA1-ED66-8A8B</v>
       </c>
       <c r="C19" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1802,11 +1939,11 @@
       </c>
       <c r="B20" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>1819-347A-5279-5B8E</v>
+        <v>51B7-BFEC-2273-E614</v>
       </c>
       <c r="C20" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1815,11 +1952,11 @@
       </c>
       <c r="B21" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>1B3C-747B-5AA-7B5A</v>
+        <v>BE81-912-6FC4-18B9</v>
       </c>
       <c r="C21" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,11 +1965,11 @@
       </c>
       <c r="B22" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>4A71-ABE1-997E-F8FF</v>
+        <v>A68C-11E9-D307-8B3C</v>
       </c>
       <c r="C22" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1841,11 +1978,11 @@
       </c>
       <c r="B23" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>81DD-7D62-FCF-5A2F</v>
+        <v>76B4-E9C8-E997-1F58</v>
       </c>
       <c r="C23" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,11 +1991,11 @@
       </c>
       <c r="B24" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>DC83-27D8-AFFD-D6AF</v>
+        <v>E637-D85B-D223-F938</v>
       </c>
       <c r="C24" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1867,11 +2004,11 @@
       </c>
       <c r="B25" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>D943-67A5-9B92-518C</v>
+        <v>506D-D5AA-820C-40A5</v>
       </c>
       <c r="C25" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1880,11 +2017,11 @@
       </c>
       <c r="B26" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>276A-A137-86B5-1CFA</v>
+        <v>B47E-3247-35A0-F4F9</v>
       </c>
       <c r="C26" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1893,11 +2030,11 @@
       </c>
       <c r="B27" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>A23-745C-7D3-3931</v>
+        <v>C930-8532-9807-37DD</v>
       </c>
       <c r="C27" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1906,11 +2043,11 @@
       </c>
       <c r="B28" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>1987-1444-5B0C-8255</v>
+        <v>99EF-BA2D-8228-47C8</v>
       </c>
       <c r="C28" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1919,11 +2056,11 @@
       </c>
       <c r="B29" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>2A72-43F7-AB17-D03</v>
+        <v>FB83-5133-7AB1-1025</v>
       </c>
       <c r="C29" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1932,11 +2069,11 @@
       </c>
       <c r="B30" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>2D46-37FF-31AA-1FC1</v>
+        <v>17F8-AE22-C5D6-4501</v>
       </c>
       <c r="C30" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,11 +2082,11 @@
       </c>
       <c r="B31" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>D678-8B84-3360-AB19</v>
+        <v>6702-AB2C-975-C446</v>
       </c>
       <c r="C31" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42754</v>
+        <v>42755</v>
       </c>
     </row>
   </sheetData>
@@ -1971,17 +2108,17 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.5465587044534"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1821862348178"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.1943319838057"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.66801619433198"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0364372469636"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5465587044534"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.6882591093117"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.78947368421053"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2058,39 +2195,39 @@
       </c>
       <c r="B3" s="3" t="n">
         <f aca="false">1+MOD(RANDBETWEEN(2,5),5)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="n">
         <f aca="false">RANDBETWEEN(100000,200000)</f>
-        <v>193925</v>
+        <v>174605</v>
       </c>
       <c r="D3" s="3" t="n">
         <f aca="false">RANDBETWEEN(1,3)+RANDBETWEEN(0,3)/10</f>
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="E3" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)))</f>
-        <v>4E-BE-5F-43-3D-4C</v>
+        <v>10-A3-DF-53-40-81</v>
       </c>
       <c r="F3" s="3" t="n">
-        <f aca="true">RAND()*15+30</f>
-        <v>38.6404883467705</v>
+        <f aca="true">ROUND(RAND()*15+30,3)</f>
+        <v>43.214</v>
       </c>
       <c r="G3" s="3" t="n">
-        <f aca="true">-(RAND()*40+80)</f>
-        <v>-99.1201749676166</v>
+        <f aca="true">ROUND(-(RAND()*40+80),3)</f>
+        <v>-80.453</v>
       </c>
       <c r="H3" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>781F-9B9-DCB9-6C73</v>
+        <v>6C28-B184-57AA-C63A</v>
       </c>
       <c r="I3" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43163.8808912738</v>
+        <v>43050.7883589601</v>
       </c>
       <c r="J3" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
@@ -2102,39 +2239,39 @@
       </c>
       <c r="B4" s="3" t="n">
         <f aca="false">1+MOD(RANDBETWEEN(2,5),5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3" t="n">
         <f aca="false">RANDBETWEEN(100000,200000)</f>
-        <v>155143</v>
+        <v>148794</v>
       </c>
       <c r="D4" s="3" t="n">
         <f aca="false">RANDBETWEEN(1,3)+RANDBETWEEN(0,3)/10</f>
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="E4" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)))</f>
-        <v>A4-50-78-BE-47-9F</v>
+        <v>F8-24-43-F9-A6-99</v>
       </c>
       <c r="F4" s="3" t="n">
-        <f aca="true">RAND()*15+30</f>
-        <v>30.4443520016667</v>
+        <f aca="true">ROUND(RAND()*15+30,3)</f>
+        <v>39.355</v>
       </c>
       <c r="G4" s="3" t="n">
-        <f aca="true">-(RAND()*40+80)</f>
-        <v>-102.394207198882</v>
+        <f aca="true">ROUND(-(RAND()*40+80),3)</f>
+        <v>-99.846</v>
       </c>
       <c r="H4" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>2F52-82B3-575B-CE91</v>
+        <v>14F4-D2CF-4E2D-65D4</v>
       </c>
       <c r="I4" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>42955.0911258699</v>
+        <v>43170.2430807717</v>
       </c>
       <c r="J4" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
-        <v>718</v>
+        <v>945</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="4"/>
@@ -2146,39 +2283,39 @@
       </c>
       <c r="B5" s="3" t="n">
         <f aca="false">1+MOD(RANDBETWEEN(2,5),5)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3" t="n">
         <f aca="false">RANDBETWEEN(100000,200000)</f>
-        <v>182849</v>
+        <v>121861</v>
       </c>
       <c r="D5" s="3" t="n">
         <f aca="false">RANDBETWEEN(1,3)+RANDBETWEEN(0,3)/10</f>
-        <v>1.1</v>
+        <v>3</v>
       </c>
       <c r="E5" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)))</f>
-        <v>B1-21-7F-7C-10-B4</v>
+        <v>44-2E-FE-5B-A0-38</v>
       </c>
       <c r="F5" s="3" t="n">
-        <f aca="true">RAND()*15+30</f>
-        <v>37.3469716625837</v>
+        <f aca="true">ROUND(RAND()*15+30,3)</f>
+        <v>30.906</v>
       </c>
       <c r="G5" s="3" t="n">
-        <f aca="true">-(RAND()*40+80)</f>
-        <v>-100.767691560924</v>
+        <f aca="true">ROUND(-(RAND()*40+80),3)</f>
+        <v>-113.632</v>
       </c>
       <c r="H5" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>34C9-4BC6-E586-16E3</v>
+        <v>A000-9DA2-84EC-85AE</v>
       </c>
       <c r="I5" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43019.0790819109</v>
+        <v>43159.3156161525</v>
       </c>
       <c r="J5" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
-        <v>890</v>
+        <v>822</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="4"/>
@@ -2190,11 +2327,11 @@
       </c>
       <c r="B6" s="3" t="n">
         <f aca="false">1+MOD(RANDBETWEEN(2,5),5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3" t="n">
         <f aca="false">RANDBETWEEN(100000,200000)</f>
-        <v>184570</v>
+        <v>137788</v>
       </c>
       <c r="D6" s="3" t="n">
         <f aca="false">RANDBETWEEN(1,3)+RANDBETWEEN(0,3)/10</f>
@@ -2202,27 +2339,27 @@
       </c>
       <c r="E6" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)))</f>
-        <v>3A-8F-BE-6A-96-16</v>
+        <v>31-45-CF-3C-FB-A9</v>
       </c>
       <c r="F6" s="3" t="n">
-        <f aca="true">RAND()*15+30</f>
-        <v>41.2687402705768</v>
+        <f aca="true">ROUND(RAND()*15+30,3)</f>
+        <v>39.902</v>
       </c>
       <c r="G6" s="3" t="n">
-        <f aca="true">-(RAND()*40+80)</f>
-        <v>-118.29945210023</v>
+        <f aca="true">ROUND(-(RAND()*40+80),3)</f>
+        <v>-98.427</v>
       </c>
       <c r="H6" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>201E-A350-F2D5-972C</v>
+        <v>36EA-A743-581E-D84</v>
       </c>
       <c r="I6" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43191.5732605391</v>
+        <v>42884.4121236989</v>
       </c>
       <c r="J6" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
-        <v>864</v>
+        <v>867</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="4"/>
@@ -2234,39 +2371,39 @@
       </c>
       <c r="B7" s="3" t="n">
         <f aca="false">1+MOD(RANDBETWEEN(2,5),5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3" t="n">
         <f aca="false">RANDBETWEEN(100000,200000)</f>
-        <v>184141</v>
+        <v>106285</v>
       </c>
       <c r="D7" s="3" t="n">
         <f aca="false">RANDBETWEEN(1,3)+RANDBETWEEN(0,3)/10</f>
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)))</f>
-        <v>B4-67-6C-E8-98-8E</v>
+        <v>5D-52-63-54-3C-1B</v>
       </c>
       <c r="F7" s="3" t="n">
-        <f aca="true">RAND()*15+30</f>
-        <v>43.1037161890804</v>
+        <f aca="true">ROUND(RAND()*15+30,3)</f>
+        <v>43.568</v>
       </c>
       <c r="G7" s="3" t="n">
-        <f aca="true">-(RAND()*40+80)</f>
-        <v>-94.1224003924868</v>
+        <f aca="true">ROUND(-(RAND()*40+80),3)</f>
+        <v>-112.986</v>
       </c>
       <c r="H7" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>7212-15E8-F941-4572</v>
+        <v>2BC3-19FD-E8CE-FF6B</v>
       </c>
       <c r="I7" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43131.4312002777</v>
+        <v>42950.8723081282</v>
       </c>
       <c r="J7" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
-        <v>800</v>
+        <v>589</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="4"/>
@@ -2278,39 +2415,39 @@
       </c>
       <c r="B8" s="3" t="n">
         <f aca="false">1+MOD(RANDBETWEEN(2,5),5)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3" t="n">
         <f aca="false">RANDBETWEEN(100000,200000)</f>
-        <v>175620</v>
+        <v>156567</v>
       </c>
       <c r="D8" s="3" t="n">
         <f aca="false">RANDBETWEEN(1,3)+RANDBETWEEN(0,3)/10</f>
-        <v>2</v>
+        <v>2.2</v>
       </c>
       <c r="E8" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)))</f>
-        <v>82-B7-2D-39-89-5B</v>
+        <v>34-55-4F-EC-43-D2</v>
       </c>
       <c r="F8" s="3" t="n">
-        <f aca="true">RAND()*15+30</f>
-        <v>35.6288181873444</v>
+        <f aca="true">ROUND(RAND()*15+30,3)</f>
+        <v>36.487</v>
       </c>
       <c r="G8" s="3" t="n">
-        <f aca="true">-(RAND()*40+80)</f>
-        <v>-118.00111512612</v>
+        <f aca="true">ROUND(-(RAND()*40+80),3)</f>
+        <v>-111.934</v>
       </c>
       <c r="H8" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>5704-6F8F-C2D3-3C60</v>
+        <v>92E0-D0A0-8A77-121</v>
       </c>
       <c r="I8" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43168.3707279928</v>
+        <v>43016.9110783804</v>
       </c>
       <c r="J8" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
-        <v>698</v>
+        <v>757</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="4"/>
@@ -2322,39 +2459,39 @@
       </c>
       <c r="B9" s="3" t="n">
         <f aca="false">1+MOD(RANDBETWEEN(2,5),5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="3" t="n">
         <f aca="false">RANDBETWEEN(100000,200000)</f>
-        <v>164524</v>
+        <v>114822</v>
       </c>
       <c r="D9" s="3" t="n">
         <f aca="false">RANDBETWEEN(1,3)+RANDBETWEEN(0,3)/10</f>
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)))</f>
-        <v>BD-60-23-2B-E7-21</v>
+        <v>B3-48-A6-E3-1D-B7</v>
       </c>
       <c r="F9" s="3" t="n">
-        <f aca="true">RAND()*15+30</f>
-        <v>36.2183278023532</v>
+        <f aca="true">ROUND(RAND()*15+30,3)</f>
+        <v>37.803</v>
       </c>
       <c r="G9" s="3" t="n">
-        <f aca="true">-(RAND()*40+80)</f>
-        <v>-110.849273279481</v>
+        <f aca="true">ROUND(-(RAND()*40+80),3)</f>
+        <v>-97.569</v>
       </c>
       <c r="H9" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>2E5B-7E62-356F-2D0F</v>
+        <v>324D-85FE-815F-D981</v>
       </c>
       <c r="I9" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43089.5416816863</v>
+        <v>43117.2365391687</v>
       </c>
       <c r="J9" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
-        <v>727</v>
+        <v>542</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="4"/>
@@ -2366,39 +2503,39 @@
       </c>
       <c r="B10" s="3" t="n">
         <f aca="false">1+MOD(RANDBETWEEN(2,5),5)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" s="3" t="n">
         <f aca="false">RANDBETWEEN(100000,200000)</f>
-        <v>102245</v>
+        <v>179072</v>
       </c>
       <c r="D10" s="3" t="n">
         <f aca="false">RANDBETWEEN(1,3)+RANDBETWEEN(0,3)/10</f>
-        <v>1.3</v>
+        <v>2.2</v>
       </c>
       <c r="E10" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)))</f>
-        <v>9C-B2-76-A1-A8-6E</v>
+        <v>92-C0-FB-B9-AB-2E</v>
       </c>
       <c r="F10" s="3" t="n">
-        <f aca="true">RAND()*15+30</f>
-        <v>34.5004548696077</v>
+        <f aca="true">ROUND(RAND()*15+30,3)</f>
+        <v>42.359</v>
       </c>
       <c r="G10" s="3" t="n">
-        <f aca="true">-(RAND()*40+80)</f>
-        <v>-116.660645137906</v>
+        <f aca="true">ROUND(-(RAND()*40+80),3)</f>
+        <v>-117.725</v>
       </c>
       <c r="H10" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>6789-D30A-9692-C681</v>
+        <v>4595-3BA8-F7B4-E46D</v>
       </c>
       <c r="I10" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43148.73055262</v>
+        <v>42956.5160013738</v>
       </c>
       <c r="J10" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
-        <v>470</v>
+        <v>528</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="4"/>
@@ -2414,35 +2551,35 @@
       </c>
       <c r="C11" s="3" t="n">
         <f aca="false">RANDBETWEEN(100000,200000)</f>
-        <v>124684</v>
+        <v>187960</v>
       </c>
       <c r="D11" s="3" t="n">
         <f aca="false">RANDBETWEEN(1,3)+RANDBETWEEN(0,3)/10</f>
-        <v>3.1</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)))</f>
-        <v>8E-FA-C8-37-80-7D</v>
+        <v>69-9B-F0-39-2F-3B</v>
       </c>
       <c r="F11" s="3" t="n">
-        <f aca="true">RAND()*15+30</f>
-        <v>33.809653526246</v>
+        <f aca="true">ROUND(RAND()*15+30,3)</f>
+        <v>32.228</v>
       </c>
       <c r="G11" s="3" t="n">
-        <f aca="true">-(RAND()*40+80)</f>
-        <v>-80.208271935643</v>
+        <f aca="true">ROUND(-(RAND()*40+80),3)</f>
+        <v>-93.54</v>
       </c>
       <c r="H11" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>38F-70AE-C814-DA7F</v>
+        <v>D9CB-1677-D9C8-EBAE</v>
       </c>
       <c r="I11" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>42885.1402188028</v>
+        <v>42986.5848303066</v>
       </c>
       <c r="J11" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
-        <v>58</v>
+        <v>535</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="4"/>
@@ -2458,35 +2595,35 @@
       </c>
       <c r="C12" s="3" t="n">
         <f aca="false">RANDBETWEEN(100000,200000)</f>
-        <v>155518</v>
+        <v>125973</v>
       </c>
       <c r="D12" s="3" t="n">
         <f aca="false">RANDBETWEEN(1,3)+RANDBETWEEN(0,3)/10</f>
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="E12" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)))</f>
-        <v>45-6C-AC-2C-CE-BC</v>
+        <v>ED-58-7A-93-27-91</v>
       </c>
       <c r="F12" s="3" t="n">
-        <f aca="true">RAND()*15+30</f>
-        <v>34.7433069535533</v>
+        <f aca="true">ROUND(RAND()*15+30,3)</f>
+        <v>43.893</v>
       </c>
       <c r="G12" s="3" t="n">
-        <f aca="true">-(RAND()*40+80)</f>
-        <v>-85.6509807716951</v>
+        <f aca="true">ROUND(-(RAND()*40+80),3)</f>
+        <v>-104.851</v>
       </c>
       <c r="H12" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>99D-3FCA-C170-254F</v>
+        <v>AA90-3E67-B339-774F</v>
       </c>
       <c r="I12" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43169.3511447476</v>
+        <v>43181.5446642436</v>
       </c>
       <c r="J12" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
-        <v>792</v>
+        <v>623</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="4"/>
@@ -2498,39 +2635,39 @@
       </c>
       <c r="B13" s="3" t="n">
         <f aca="false">1+MOD(RANDBETWEEN(2,5),5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="3" t="n">
         <f aca="false">RANDBETWEEN(100000,200000)</f>
-        <v>175032</v>
+        <v>176475</v>
       </c>
       <c r="D13" s="3" t="n">
         <f aca="false">RANDBETWEEN(1,3)+RANDBETWEEN(0,3)/10</f>
-        <v>1</v>
+        <v>3.1</v>
       </c>
       <c r="E13" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)),"-",DEC2HEX(RANDBETWEEN(16,255)))</f>
-        <v>1D-85-8D-18-E2-AC</v>
+        <v>C6-8C-E3-4F-AC-3F</v>
       </c>
       <c r="F13" s="3" t="n">
-        <f aca="true">RAND()*15+30</f>
-        <v>32.8746284467939</v>
+        <f aca="true">ROUND(RAND()*15+30,3)</f>
+        <v>44.204</v>
       </c>
       <c r="G13" s="3" t="n">
-        <f aca="true">-(RAND()*40+80)</f>
-        <v>-102.696371925404</v>
+        <f aca="true">ROUND(-(RAND()*40+80),3)</f>
+        <v>-104.674</v>
       </c>
       <c r="H13" s="3" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)),"-",DEC2HEX(RANDBETWEEN(0,65535)))</f>
-        <v>1501-D323-9C66-B048</v>
+        <v>BFE2-F261-6C09-5CC9</v>
       </c>
       <c r="I13" s="5" t="n">
         <f aca="true">NOW()+100 + RAND()*365</f>
-        <v>43070.7305775495</v>
+        <v>43011.2346258283</v>
       </c>
       <c r="J13" s="3" t="n">
         <f aca="false">RANDBETWEEN(0,1000)</f>
-        <v>921</v>
+        <v>541</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="4"/>
@@ -2594,14 +2731,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="25.2145748987854"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="11.753036437247"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="6" width="16.5263157894737"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.66801619433198"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="25.82995951417"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.4048582995951"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="6" width="16.8947368421053"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.78947368421053"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4007,15 +4144,15 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1821862348178"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.66801619433198"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.78947368421053"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4070,91 +4207,94 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>1433-9F03</v>
+        <v>CDB7-DE19</v>
       </c>
       <c r="C3" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>27644.6630916277</v>
+        <v>39775.207877739</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>175</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>28</v>
+        <v>176</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
       <c r="G3" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
         <v>4</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0" t="str">
+        <f aca="false">CONCATENATE(E3, ".",F4,"@patient.com")</f>
+        <v>Nathalia.Fisher@patient.com</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>7799-AF39</v>
+        <v>E0F3-6A0A</v>
       </c>
       <c r="C4" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>40916.0518702066</v>
+        <v>10247.4740518046</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>175</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>28</v>
+        <v>178</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>131</v>
+        <v>179</v>
       </c>
       <c r="G4" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
         <v>3</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="str">
+        <f aca="false">CONCATENATE(E4, ".",F5,"@patient.com")</f>
+        <v>Grace.Bartlett@patient.com</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>C8CE-C6C3</v>
+        <v>3066-3F17</v>
       </c>
       <c r="C5" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>20814.9597363662</v>
+        <v>21788.2860849428</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>175</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>28</v>
+        <v>180</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
         <v>3</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>132</v>
+      <c r="H5" s="0" t="str">
+        <f aca="false">CONCATENATE(E5, ".",F6,"@patient.com")</f>
+        <v>Lucille.George@patient.com</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4163,24 +4303,24 @@
       </c>
       <c r="B6" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>E7E5-103D</v>
+        <v>B865-9BB1</v>
       </c>
       <c r="C6" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>35266.0770189259</v>
+        <v>25392.4437426164</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>175</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>135</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6" s="0" t="str">
         <f aca="false">CONCATENATE(E6, ".",F7,"@patient.com")</f>
@@ -4193,20 +4333,20 @@
       </c>
       <c r="B7" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>8AEA-8FC8</v>
+        <v>FBC8-89E2</v>
       </c>
       <c r="C7" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>41198.1425958285</v>
+        <v>37019.5141304948</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>175</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -4223,20 +4363,20 @@
       </c>
       <c r="B8" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>C80E-7060</v>
+        <v>9345-43CA</v>
       </c>
       <c r="C8" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>13689.6161005364</v>
+        <v>23030.9059321257</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>175</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -4253,20 +4393,20 @@
       </c>
       <c r="B9" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>F7F4-3D6D</v>
+        <v>BD85-C350</v>
       </c>
       <c r="C9" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>25478.2228110151</v>
+        <v>25376.3575476065</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>175</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -4283,24 +4423,24 @@
       </c>
       <c r="B10" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>40EB-6316</v>
+        <v>3A05-A02D</v>
       </c>
       <c r="C10" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>27914.7109799274</v>
+        <v>38297.5436083537</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>175</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H10" s="0" t="str">
         <f aca="false">CONCATENATE(E10, ".",F11,"@patient.com")</f>
@@ -4313,20 +4453,20 @@
       </c>
       <c r="B11" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>FAD9-CC7F</v>
+        <v>94BC-FACB</v>
       </c>
       <c r="C11" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>12971.0942591532</v>
+        <v>12269.1799538849</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>175</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -4343,24 +4483,24 @@
       </c>
       <c r="B12" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>E80E-5E9D</v>
+        <v>F850-34A0</v>
       </c>
       <c r="C12" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>34685.2984233495</v>
+        <v>42664.3215446216</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>175</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>142</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H12" s="0" t="str">
         <f aca="false">CONCATENATE(E12, ".",F13,"@patient.com")</f>
@@ -4373,20 +4513,20 @@
       </c>
       <c r="B13" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>CEFF-E388</v>
+        <v>6AD3-3F21</v>
       </c>
       <c r="C13" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>32194.485018603</v>
+        <v>23456.9147372753</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>175</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -4403,20 +4543,20 @@
       </c>
       <c r="B14" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>744E-CF63</v>
+        <v>3A96-44BE</v>
       </c>
       <c r="C14" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>26020.9312368342</v>
+        <v>27512.9577934871</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -4433,24 +4573,24 @@
       </c>
       <c r="B15" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>E4F2-CDE0</v>
+        <v>5FA5-B6EC</v>
       </c>
       <c r="C15" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>25910.4683461204</v>
+        <v>33550.5735512863</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="G15" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H15" s="0" t="str">
         <f aca="false">CONCATENATE(E15, ".",F16,"@patient.com")</f>
@@ -4463,24 +4603,24 @@
       </c>
       <c r="B16" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>FF18-CF36</v>
+        <v>7063-6F85</v>
       </c>
       <c r="C16" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>33332.6757615986</v>
+        <v>32851.9518937586</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H16" s="0" t="str">
         <f aca="false">CONCATENATE(E16, ".",F17,"@patient.com")</f>
@@ -4493,20 +4633,20 @@
       </c>
       <c r="B17" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>5D40-5F50</v>
+        <v>FE68-37F6</v>
       </c>
       <c r="C17" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>21605.1605578478</v>
+        <v>12923.6084256194</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="G17" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -4523,20 +4663,20 @@
       </c>
       <c r="B18" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>EB8E-FF15</v>
+        <v>DD31-4F9A</v>
       </c>
       <c r="C18" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>20972.3497569664</v>
+        <v>32152.0539834419</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="G18" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -4553,20 +4693,20 @@
       </c>
       <c r="B19" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>C345-514C</v>
+        <v>FD87-E798</v>
       </c>
       <c r="C19" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>17960.4940032943</v>
+        <v>18345.1412830965</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="G19" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -4583,24 +4723,24 @@
       </c>
       <c r="B20" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>F7A6-AEE7</v>
+        <v>9C23-4251</v>
       </c>
       <c r="C20" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>34335.8426913485</v>
+        <v>24190.2889408012</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="G20" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H20" s="0" t="str">
         <f aca="false">CONCATENATE(E20, ".",F21,"@patient.com")</f>
@@ -4613,20 +4753,20 @@
       </c>
       <c r="B21" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>344D-25BF</v>
+        <v>6DBC-DAD9</v>
       </c>
       <c r="C21" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>31975.2258304858</v>
+        <v>17060.0782099594</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="G21" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -4643,24 +4783,24 @@
       </c>
       <c r="B22" s="0" t="str">
         <f aca="false">CONCATENATE(DEC2HEX(RANDBETWEEN(4096,65535)),"-",DEC2HEX(RANDBETWEEN(4096,65535)))</f>
-        <v>4E64-14C1</v>
+        <v>1670-117C</v>
       </c>
       <c r="C22" s="12" t="n">
         <f aca="true">NOW()-90*365*RAND()</f>
-        <v>36108.5551310697</v>
+        <v>32883.1955790694</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="G22" s="0" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H22" s="0" t="str">
         <f aca="false">CONCATENATE(E22, ".",F23,"@patient.com")</f>
@@ -4668,11 +4808,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" display="patient1@patient.com"/>
-    <hyperlink ref="H4" r:id="rId2" display="patient2@patient.com"/>
-    <hyperlink ref="H5" r:id="rId3" display="patient3@patient.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4691,15 +4826,15 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="6" width="9.54655870445344"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="23.3805668016194"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="23.3805668016194"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.66801619433198"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="6" width="9.66801619433198"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="23.8744939271255"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="0" width="23.8744939271255"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.78947368421053"/>
   </cols>
   <sheetData>
     <row r="1" s="16" customFormat="true" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4707,25 +4842,25 @@
         <v>10</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>100</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>18</v>
@@ -4754,7 +4889,7 @@
         <v>110</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>2</v>
@@ -4766,34 +4901,34 @@
       </c>
       <c r="B3" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C3" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <f aca="false">1+RANDBETWEEN(1,10)</f>
         <v>10</v>
-      </c>
-      <c r="F3" s="6" t="n">
-        <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>6</v>
       </c>
       <c r="G3" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>1.34</v>
+        <v>7.148</v>
       </c>
       <c r="H3" s="17" t="n">
         <f aca="true">NOW() -RAND()*99.7</f>
-        <v>42746.6334873178</v>
+        <v>42723.6891987837</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4802,7 +4937,7 @@
       </c>
       <c r="B4" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
@@ -4810,26 +4945,26 @@
       </c>
       <c r="D4" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F4" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G4" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>1.511</v>
+        <v>9.34</v>
       </c>
       <c r="H4" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42734.9398483224</v>
+        <v>42713.1407347243</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
@@ -4840,34 +4975,34 @@
       </c>
       <c r="B5" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F5" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G5" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>8.288</v>
+        <v>3.887</v>
       </c>
       <c r="H5" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42686.0418299214</v>
+        <v>42682.2765693108</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
@@ -4878,7 +5013,7 @@
       </c>
       <c r="B6" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
@@ -4886,26 +5021,26 @@
       </c>
       <c r="D6" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F6" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G6" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>8.932</v>
+        <v>9.852</v>
       </c>
       <c r="H6" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42692.273164129</v>
+        <v>42698.7518229751</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
@@ -4916,11 +5051,11 @@
       </c>
       <c r="B7" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -4928,22 +5063,22 @@
       </c>
       <c r="E7" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F7" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G7" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>5.382</v>
+        <v>1.347</v>
       </c>
       <c r="H7" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42721.3897407515</v>
+        <v>42656.8748782841</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
@@ -4954,34 +5089,34 @@
       </c>
       <c r="B8" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C8" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E8" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F8" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G8" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>6.998</v>
+        <v>8.324</v>
       </c>
       <c r="H8" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42719.1762588992</v>
+        <v>42742.4803643381</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -4992,7 +5127,7 @@
       </c>
       <c r="B9" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
@@ -5004,22 +5139,22 @@
       </c>
       <c r="E9" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F9" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>7.483</v>
+        <v>7.603</v>
       </c>
       <c r="H9" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42660.9190820414</v>
+        <v>42674.7581719724</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
@@ -5030,11 +5165,11 @@
       </c>
       <c r="B10" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C10" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -5042,22 +5177,22 @@
       </c>
       <c r="E10" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>8.502</v>
+        <v>9.589</v>
       </c>
       <c r="H10" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42658.5776522679</v>
+        <v>42754.6908006496</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
@@ -5068,7 +5203,7 @@
       </c>
       <c r="B11" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C11" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
@@ -5076,7 +5211,7 @@
       </c>
       <c r="D11" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
@@ -5084,18 +5219,18 @@
       </c>
       <c r="F11" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G11" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>3.376</v>
+        <v>1.295</v>
       </c>
       <c r="H11" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42705.3409825273</v>
+        <v>42683.9561998356</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
@@ -5110,30 +5245,30 @@
       </c>
       <c r="C12" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D12" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G12" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>8.618</v>
+        <v>3.255</v>
       </c>
       <c r="H12" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42753.7996062784</v>
+        <v>42740.8688985807</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
@@ -5144,11 +5279,11 @@
       </c>
       <c r="B13" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C13" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D13" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -5156,22 +5291,22 @@
       </c>
       <c r="E13" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F13" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G13" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>2.74</v>
+        <v>5.929</v>
       </c>
       <c r="H13" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42680.0159384553</v>
+        <v>42665.3457921612</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
@@ -5182,7 +5317,7 @@
       </c>
       <c r="B14" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C14" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
@@ -5194,22 +5329,22 @@
       </c>
       <c r="E14" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F14" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G14" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>0.232</v>
+        <v>0.493</v>
       </c>
       <c r="H14" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42705.0074789912</v>
+        <v>42658.8545524769</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
@@ -5220,7 +5355,7 @@
       </c>
       <c r="B15" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C15" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
@@ -5228,26 +5363,26 @@
       </c>
       <c r="D15" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E15" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F15" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>3.182</v>
+        <v>6.648</v>
       </c>
       <c r="H15" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42692.1621773603</v>
+        <v>42736.4436902852</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
@@ -5258,7 +5393,7 @@
       </c>
       <c r="B16" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C16" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
@@ -5266,11 +5401,11 @@
       </c>
       <c r="D16" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F16" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
@@ -5278,14 +5413,14 @@
       </c>
       <c r="G16" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>8.283</v>
+        <v>0.04</v>
       </c>
       <c r="H16" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42667.3267370543</v>
+        <v>42678.7856624411</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
@@ -5296,7 +5431,7 @@
       </c>
       <c r="B17" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C17" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
@@ -5304,26 +5439,26 @@
       </c>
       <c r="D17" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
+        <v>3</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <f aca="false">1+RANDBETWEEN(1,10)</f>
+        <v>2</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <f aca="false">1+RANDBETWEEN(1,10)</f>
         <v>4</v>
-      </c>
-      <c r="E17" s="6" t="n">
-        <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>5</v>
-      </c>
-      <c r="F17" s="6" t="n">
-        <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>3</v>
       </c>
       <c r="G17" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>6.758</v>
+        <v>7.95</v>
       </c>
       <c r="H17" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42702.9018386195</v>
+        <v>42679.4634066311</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
@@ -5334,11 +5469,11 @@
       </c>
       <c r="B18" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C18" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -5350,18 +5485,18 @@
       </c>
       <c r="F18" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G18" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>1.91</v>
+        <v>3.306</v>
       </c>
       <c r="H18" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42728.0315693796</v>
+        <v>42657.3990312735</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
@@ -5372,34 +5507,34 @@
       </c>
       <c r="B19" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C19" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F19" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G19" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>6.057</v>
+        <v>5.943</v>
       </c>
       <c r="H19" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42667.0599915027</v>
+        <v>42699.6300553981</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
@@ -5410,34 +5545,34 @@
       </c>
       <c r="B20" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C20" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D20" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
+        <v>3</v>
+      </c>
+      <c r="F20" s="6" t="n">
+        <f aca="false">1+RANDBETWEEN(1,10)</f>
         <v>9</v>
-      </c>
-      <c r="F20" s="6" t="n">
-        <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>3</v>
       </c>
       <c r="G20" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>2.838</v>
+        <v>8.927</v>
       </c>
       <c r="H20" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42716.6479298074</v>
+        <v>42659.9993265992</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
@@ -5448,7 +5583,7 @@
       </c>
       <c r="B21" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C21" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
@@ -5456,26 +5591,26 @@
       </c>
       <c r="D21" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E21" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F21" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G21" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>8.618</v>
+        <v>4.957</v>
       </c>
       <c r="H21" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42675.7470376414</v>
+        <v>42754.9951909326</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
@@ -5486,7 +5621,7 @@
       </c>
       <c r="B22" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C22" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
@@ -5498,7 +5633,7 @@
       </c>
       <c r="E22" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
@@ -5506,14 +5641,14 @@
       </c>
       <c r="G22" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>4.171</v>
+        <v>7.811</v>
       </c>
       <c r="H22" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42699.6975815463</v>
+        <v>42716.4016980217</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
@@ -5524,34 +5659,34 @@
       </c>
       <c r="B23" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C23" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E23" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F23" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G23" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>4.582</v>
+        <v>5.458</v>
       </c>
       <c r="H23" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42674.6548139544</v>
+        <v>42738.2341130915</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
@@ -5562,15 +5697,15 @@
       </c>
       <c r="B24" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C24" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E24" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
@@ -5578,18 +5713,18 @@
       </c>
       <c r="F24" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G24" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>2.397</v>
+        <v>7.683</v>
       </c>
       <c r="H24" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42721.9937511187</v>
+        <v>42693.7130612852</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -5600,7 +5735,7 @@
       </c>
       <c r="B25" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C25" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
@@ -5608,26 +5743,26 @@
       </c>
       <c r="D25" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E25" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F25" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G25" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>1.979</v>
+        <v>3.501</v>
       </c>
       <c r="H25" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42703.7337144174</v>
+        <v>42669.1265946903</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
@@ -5638,34 +5773,34 @@
       </c>
       <c r="B26" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C26" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D26" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
+        <v>3</v>
+      </c>
+      <c r="E26" s="6" t="n">
+        <f aca="false">1+RANDBETWEEN(1,10)</f>
+        <v>8</v>
+      </c>
+      <c r="F26" s="6" t="n">
+        <f aca="false">1+RANDBETWEEN(1,10)</f>
         <v>4</v>
-      </c>
-      <c r="E26" s="6" t="n">
-        <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>9</v>
-      </c>
-      <c r="F26" s="6" t="n">
-        <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>10</v>
       </c>
       <c r="G26" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>7.148</v>
+        <v>9.543</v>
       </c>
       <c r="H26" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42724.7060057481</v>
+        <v>42693.175357516</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
@@ -5688,22 +5823,22 @@
       </c>
       <c r="E27" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F27" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G27" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>3.899</v>
+        <v>3.387</v>
       </c>
       <c r="H27" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42735.1121900129</v>
+        <v>42748.1961901762</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -5714,34 +5849,34 @@
       </c>
       <c r="B28" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D28" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E28" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F28" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G28" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>4.702</v>
+        <v>4.054</v>
       </c>
       <c r="H28" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42747.3262016465</v>
+        <v>42672.2244881388</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
@@ -5752,34 +5887,34 @@
       </c>
       <c r="B29" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C29" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D29" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E29" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F29" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G29" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>8.673</v>
+        <v>0.422</v>
       </c>
       <c r="H29" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42685.9906537457</v>
+        <v>42689.9992655369</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
@@ -5790,7 +5925,7 @@
       </c>
       <c r="B30" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C30" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
@@ -5798,26 +5933,26 @@
       </c>
       <c r="D30" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
+        <v>4</v>
+      </c>
+      <c r="E30" s="6" t="n">
+        <f aca="false">1+RANDBETWEEN(1,10)</f>
+        <v>3</v>
+      </c>
+      <c r="F30" s="6" t="n">
+        <f aca="false">1+RANDBETWEEN(1,10)</f>
         <v>5</v>
-      </c>
-      <c r="E30" s="6" t="n">
-        <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>8</v>
-      </c>
-      <c r="F30" s="6" t="n">
-        <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>10</v>
       </c>
       <c r="G30" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>8.379</v>
+        <v>2.762</v>
       </c>
       <c r="H30" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42719.178987277</v>
+        <v>42661.2972149472</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
@@ -5832,30 +5967,30 @@
       </c>
       <c r="C31" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E31" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F31" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G31" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>7.81</v>
+        <v>4.055</v>
       </c>
       <c r="H31" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42695.7204247071</v>
+        <v>42719.7713783271</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
@@ -5866,15 +6001,15 @@
       </c>
       <c r="B32" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C32" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D32" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E32" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
@@ -5886,14 +6021,14 @@
       </c>
       <c r="G32" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>7.332</v>
+        <v>1.316</v>
       </c>
       <c r="H32" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42657.701646891</v>
+        <v>42738.5287158647</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
@@ -5908,7 +6043,7 @@
       </c>
       <c r="C33" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D33" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
@@ -5916,22 +6051,22 @@
       </c>
       <c r="E33" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F33" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G33" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>9.221</v>
+        <v>4.808</v>
       </c>
       <c r="H33" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42694.6918416679</v>
+        <v>42659.0462499308</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
@@ -5942,34 +6077,34 @@
       </c>
       <c r="B34" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C34" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D34" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
+        <v>4</v>
+      </c>
+      <c r="E34" s="6" t="n">
+        <f aca="false">1+RANDBETWEEN(1,10)</f>
+        <v>10</v>
+      </c>
+      <c r="F34" s="6" t="n">
+        <f aca="false">1+RANDBETWEEN(1,10)</f>
         <v>5</v>
-      </c>
-      <c r="E34" s="6" t="n">
-        <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>8</v>
-      </c>
-      <c r="F34" s="6" t="n">
-        <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>10</v>
       </c>
       <c r="G34" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>2.828</v>
+        <v>4.173</v>
       </c>
       <c r="H34" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42729.3316881933</v>
+        <v>42672.3450494495</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
@@ -5980,37 +6115,339 @@
       </c>
       <c r="B35" s="6" t="n">
         <f aca="false">8+RANDBETWEEN(0,2)*4 + RANDBETWEEN(0,2)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C35" s="6" t="n">
         <f aca="false">RANDBETWEEN(4,6)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D35" s="6" t="n">
         <f aca="false">RANDBETWEEN(3,5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E35" s="6" t="n">
         <f aca="false">1+RANDBETWEEN(1,10)</f>
+        <v>6</v>
+      </c>
+      <c r="F35" s="6" t="n">
+        <f aca="false">1+RANDBETWEEN(1,10)</f>
         <v>3</v>
-      </c>
-      <c r="F35" s="6" t="n">
-        <f aca="false">1+RANDBETWEEN(1,10)</f>
-        <v>10</v>
       </c>
       <c r="G35" s="6" t="n">
         <f aca="false">RANDBETWEEN(1,10000)/1000</f>
-        <v>8.624</v>
+        <v>3.206</v>
       </c>
       <c r="H35" s="17" t="n">
         <f aca="true">NOW() -RAND()*100</f>
-        <v>42732.3831633681</v>
+        <v>42658.2715915943</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="31"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="13.9838056680162"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="18" width="28.085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="18" width="11.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="18" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="19" customFormat="true" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3805668016194"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.4089068825911"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B8" s="21" t="n">
+        <v>12341234</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>